<commit_message>
Streamlined QoQ Evaluation Module
</commit_message>
<xml_diff>
--- a/0_1_Output_Data/4_naive_forecaster_qoq_error_series/AVERAGE_10_6_qoq_errors_first_eval.xlsx
+++ b/0_1_Output_Data/4_naive_forecaster_qoq_error_series/AVERAGE_10_6_qoq_errors_first_eval.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>Q0</t>
   </si>
@@ -37,66 +37,354 @@
     <t>Q6</t>
   </si>
   <si>
+    <t>1988-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1989-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1989-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1989-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1989-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1990-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1990-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1990-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1990-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1991-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1991-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1991-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1991-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1992-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1992-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1992-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1992-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1993-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1993-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1993-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1993-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1994-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1994-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1994-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1994-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1995-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1995-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1995-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1995-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1996-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1996-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1996-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1996-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1997-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1997-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1997-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1997-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1998-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1998-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1998-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1998-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1999-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1999-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1999-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>1999-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2000-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2000-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2000-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2000-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2001-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2001-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2001-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2001-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2002-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2002-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2002-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2002-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2003-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2003-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2003-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2003-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2004-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2004-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2004-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2004-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2005-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2005-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2005-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2005-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2006-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2006-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2006-07-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2006-10-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2007-01-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2007-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2007-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2007-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2008-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2008-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2008-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2008-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2009-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2009-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2009-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2009-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2010-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2010-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2010-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2010-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2011-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2011-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2011-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2011-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2012-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2012-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2012-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2012-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2013-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2013-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2013-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2013-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2014-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2014-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2014-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2014-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2015-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2015-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2015-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2015-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2016-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2016-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2016-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2016-10-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2017-01-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2017-04-01 00:00:00_diff</t>
   </si>
   <si>
+    <t>2017-07-01 00:00:00_diff</t>
+  </si>
+  <si>
     <t>2017-10-01 00:00:00_diff</t>
   </si>
   <si>
@@ -188,6 +476,9 @@
   </si>
   <si>
     <t>2025-04-01 00:00:00_diff</t>
+  </si>
+  <si>
+    <t>2025-07-01 00:00:00_diff</t>
   </si>
 </sst>
 </file>
@@ -545,7 +836,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -579,25 +870,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.3963761775604042</v>
+        <v>-0.5060068269423215</v>
       </c>
       <c r="C2">
-        <v>-0.8656134284117374</v>
+        <v>-0.3315181088272636</v>
       </c>
       <c r="D2">
-        <v>1.158194699184626</v>
+        <v>0.281686368590394</v>
       </c>
       <c r="E2">
-        <v>1.186843519996163</v>
+        <v>-0.206351016835529</v>
       </c>
       <c r="F2">
-        <v>2.770372346455781</v>
+        <v>-0.4801372992501425</v>
       </c>
       <c r="G2">
-        <v>4.463193234397496</v>
+        <v>-1.379538488323946</v>
       </c>
       <c r="H2">
-        <v>0.3449098147915402</v>
+        <v>0.208980406201245</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -605,25 +896,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1.239931507228801</v>
+        <v>-0.3278447767506646</v>
       </c>
       <c r="C3">
-        <v>1.268580328040338</v>
+        <v>0.285359700666993</v>
       </c>
       <c r="D3">
-        <v>2.852109154499956</v>
+        <v>-0.20267768475893</v>
       </c>
       <c r="E3">
-        <v>4.544930042441671</v>
+        <v>-0.4764639671735434</v>
       </c>
       <c r="F3">
-        <v>0.4266466228357149</v>
+        <v>-1.375865156247347</v>
       </c>
       <c r="G3">
-        <v>0.01612894727267156</v>
+        <v>0.212653738277844</v>
       </c>
       <c r="H3">
-        <v>0.7346596165289111</v>
+        <v>-1.414454807235176</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -631,25 +922,25 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>2.646269414624167</v>
+        <v>0.3141167314837554</v>
       </c>
       <c r="C4">
-        <v>4.339090302565882</v>
+        <v>-0.1739206539421676</v>
       </c>
       <c r="D4">
-        <v>0.2208068829599255</v>
+        <v>-0.447706936356781</v>
       </c>
       <c r="E4">
-        <v>-0.1897107926031179</v>
+        <v>-1.347108125430584</v>
       </c>
       <c r="F4">
-        <v>0.5288198766531217</v>
+        <v>0.2414107690946064</v>
       </c>
       <c r="G4">
-        <v>0.3769767350323958</v>
+        <v>-1.385697776418413</v>
       </c>
       <c r="H4">
-        <v>-1.643763506744272</v>
+        <v>-1.046496365682932</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -657,25 +948,25 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-0.5974898394390895</v>
+        <v>-0.2315013303517287</v>
       </c>
       <c r="C5">
-        <v>-1.008007515002133</v>
+        <v>-0.5052876127663422</v>
       </c>
       <c r="D5">
-        <v>-0.2894768457458933</v>
+        <v>-1.404688801840145</v>
       </c>
       <c r="E5">
-        <v>-0.4413199873666193</v>
+        <v>0.1838300926850453</v>
       </c>
       <c r="F5">
-        <v>-2.462060229143287</v>
+        <v>-1.443278452827974</v>
       </c>
       <c r="G5">
-        <v>-0.977984595383529</v>
+        <v>-1.104077042092493</v>
       </c>
       <c r="H5">
-        <v>-0.6447655124219993</v>
+        <v>-2.089447838049735</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -683,25 +974,25 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-0.2939646841069006</v>
+        <v>-0.1638482841896709</v>
       </c>
       <c r="C6">
-        <v>-0.4458078257276266</v>
+        <v>-1.063249473263474</v>
       </c>
       <c r="D6">
-        <v>-2.466548067504295</v>
+        <v>0.5252694212617166</v>
       </c>
       <c r="E6">
-        <v>-0.9824724337445363</v>
+        <v>-1.101839124251303</v>
       </c>
       <c r="F6">
-        <v>-0.6492533507830067</v>
+        <v>-0.762637713515822</v>
       </c>
       <c r="G6">
-        <v>-1.783638533379176</v>
+        <v>-1.748008509473064</v>
       </c>
       <c r="H6">
-        <v>-0.4036785729014095</v>
+        <v>-0.103205209371902</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -709,25 +1000,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>-2.542893978309402</v>
+        <v>-1.170814798143758</v>
       </c>
       <c r="C7">
-        <v>-1.058818344549643</v>
+        <v>0.4177040963814331</v>
       </c>
       <c r="D7">
-        <v>-0.7255992615881137</v>
+        <v>-1.209404449131587</v>
       </c>
       <c r="E7">
-        <v>-1.859984444184283</v>
+        <v>-0.8702030383961055</v>
       </c>
       <c r="F7">
-        <v>-0.4800244837065165</v>
+        <v>-1.855573834353347</v>
       </c>
       <c r="G7">
-        <v>-0.8638202886166834</v>
+        <v>-0.2107705342521855</v>
       </c>
       <c r="H7">
-        <v>-0.1789343978423749</v>
+        <v>1.5023168425997</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -735,25 +1026,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.5351204465965399</v>
+        <v>0.5539801895018386</v>
       </c>
       <c r="C8">
-        <v>-1.66950562919271</v>
+        <v>-1.073128356011181</v>
       </c>
       <c r="D8">
-        <v>-0.2895456687149427</v>
+        <v>-0.7339269452757</v>
       </c>
       <c r="E8">
-        <v>-0.6733414736251095</v>
+        <v>-1.719297741232942</v>
       </c>
       <c r="F8">
-        <v>0.0115444171491989</v>
+        <v>-0.07449444113178005</v>
       </c>
       <c r="G8">
-        <v>-0.6804809672324722</v>
+        <v>1.638592935720106</v>
       </c>
       <c r="H8">
-        <v>-0.4410326232298434</v>
+        <v>0.1695574827230395</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -761,25 +1052,25 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.01136921538350649</v>
+        <v>-1.182597298227241</v>
       </c>
       <c r="C9">
-        <v>-0.3724265895266604</v>
+        <v>-0.84339588749176</v>
       </c>
       <c r="D9">
-        <v>0.3124593012476481</v>
+        <v>-1.828766683449002</v>
       </c>
       <c r="E9">
-        <v>-0.3795660831340231</v>
+        <v>-0.18396338334784</v>
       </c>
       <c r="F9">
-        <v>-0.1401177391313942</v>
+        <v>1.529123993504046</v>
       </c>
       <c r="G9">
-        <v>-0.1033897623722235</v>
+        <v>0.06008854050697954</v>
       </c>
       <c r="H9">
-        <v>0.723104312015092</v>
+        <v>-0.4190670429915799</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -787,25 +1078,25 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.9526635850093691</v>
+        <v>-0.5428259771141501</v>
       </c>
       <c r="C10">
-        <v>0.2606382006276979</v>
+        <v>-1.528196773071392</v>
       </c>
       <c r="D10">
-        <v>0.5000865446303268</v>
+        <v>0.1166065270297698</v>
       </c>
       <c r="E10">
-        <v>0.5368145213894975</v>
+        <v>1.829693903881656</v>
       </c>
       <c r="F10">
-        <v>1.363308595776813</v>
+        <v>0.3606584508845894</v>
       </c>
       <c r="G10">
-        <v>0.7075103856552477</v>
+        <v>-0.1184971326139701</v>
       </c>
       <c r="H10">
-        <v>0.0493601459296269</v>
+        <v>1.27138157745411</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -813,25 +1104,25 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.4274989419678774</v>
+        <v>-1.532861758448916</v>
       </c>
       <c r="C11">
-        <v>0.4642269187270481</v>
+        <v>0.111941541652246</v>
       </c>
       <c r="D11">
-        <v>1.290720993114364</v>
+        <v>1.825028918504132</v>
       </c>
       <c r="E11">
-        <v>0.6349227829927984</v>
+        <v>0.3559934655070656</v>
       </c>
       <c r="F11">
-        <v>-0.02322745673282245</v>
+        <v>-0.1231621179914939</v>
       </c>
       <c r="G11">
-        <v>0.3758874911189606</v>
+        <v>1.266716592076587</v>
       </c>
       <c r="H11">
-        <v>0.3144509489973832</v>
+        <v>1.37653315448771</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -839,25 +1130,25 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>1.235029948750828</v>
+        <v>0.2779295113485429</v>
       </c>
       <c r="C12">
-        <v>0.5792317386292632</v>
+        <v>1.991016888200429</v>
       </c>
       <c r="D12">
-        <v>-0.07891850109635756</v>
+        <v>0.5219814352033625</v>
       </c>
       <c r="E12">
-        <v>0.3201964467554255</v>
+        <v>0.04282585170480302</v>
       </c>
       <c r="F12">
-        <v>0.2587599046338481</v>
+        <v>1.432704561772884</v>
       </c>
       <c r="G12">
-        <v>-0.1754060304832554</v>
+        <v>1.542521124184007</v>
       </c>
       <c r="H12">
-        <v>0.8033953615958215</v>
+        <v>1.52900369726823</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -865,25 +1156,25 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>-0.4329776612703231</v>
+        <v>1.982365627949434</v>
       </c>
       <c r="C13">
-        <v>-0.03386271341853997</v>
+        <v>0.5133301749523675</v>
       </c>
       <c r="D13">
-        <v>-0.09529925554011737</v>
+        <v>0.03417459145380808</v>
       </c>
       <c r="E13">
-        <v>-0.529465190657221</v>
+        <v>1.424053301521889</v>
       </c>
       <c r="F13">
-        <v>0.449336201421856</v>
+        <v>1.533869863933012</v>
       </c>
       <c r="G13">
-        <v>0.2222202969739298</v>
+        <v>1.520352437017235</v>
       </c>
       <c r="H13">
-        <v>-0.4112394324521587</v>
+        <v>3.172296631159906</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -891,25 +1182,25 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>-0.1856174723396913</v>
+        <v>0.3508190488276905</v>
       </c>
       <c r="C14">
-        <v>-0.6197834074567948</v>
+        <v>-0.1283365346708689</v>
       </c>
       <c r="D14">
-        <v>0.3590179846222821</v>
+        <v>1.261542175397212</v>
       </c>
       <c r="E14">
-        <v>0.1319020801743559</v>
+        <v>1.371358737808335</v>
       </c>
       <c r="F14">
-        <v>-0.5015576492517326</v>
+        <v>1.357841310892558</v>
       </c>
       <c r="G14">
-        <v>-0.07416069059612829</v>
+        <v>3.009785505035229</v>
       </c>
       <c r="H14">
-        <v>-0.2404976452842752</v>
+        <v>0.5896905030795416</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -917,25 +1208,25 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.4273407187267424</v>
+        <v>-0.08262366775407393</v>
       </c>
       <c r="C15">
-        <v>0.2002248142788162</v>
+        <v>1.307255042314007</v>
       </c>
       <c r="D15">
-        <v>-0.4332349151472724</v>
+        <v>1.41707160472513</v>
       </c>
       <c r="E15">
-        <v>-0.005837956491668017</v>
+        <v>1.403554177809353</v>
       </c>
       <c r="F15">
-        <v>-0.1721749111798149</v>
+        <v>3.055498371952024</v>
       </c>
       <c r="G15">
-        <v>-0.0494638947389891</v>
+        <v>0.6354033699963366</v>
       </c>
       <c r="H15">
-        <v>-0.002230158183848807</v>
+        <v>0.5418631498489003</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -943,25 +1234,25 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>-0.5318964931771777</v>
+        <v>1.352079729038064</v>
       </c>
       <c r="C16">
-        <v>-0.1044995345215733</v>
+        <v>1.461896291449188</v>
       </c>
       <c r="D16">
-        <v>-0.2708364892097202</v>
+        <v>1.448378864533411</v>
       </c>
       <c r="E16">
-        <v>-0.1481254727688944</v>
+        <v>3.100323058676082</v>
       </c>
       <c r="F16">
-        <v>-0.1008917362137541</v>
+        <v>0.6802280567203944</v>
       </c>
       <c r="G16">
-        <v>-0.4975104677362057</v>
+        <v>0.5866878365729581</v>
       </c>
       <c r="H16">
-        <v>-0.2434584326124856</v>
+        <v>1.504505890656316</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -969,25 +1260,25 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>-0.1938269109680474</v>
+        <v>1.340354478924977</v>
       </c>
       <c r="C17">
-        <v>-0.07111589452722158</v>
+        <v>1.3268370520092</v>
       </c>
       <c r="D17">
-        <v>-0.02388215797208129</v>
+        <v>2.978781246151871</v>
       </c>
       <c r="E17">
-        <v>-0.4205008894945329</v>
+        <v>0.5586862441961835</v>
       </c>
       <c r="F17">
-        <v>-0.1664488543708128</v>
+        <v>0.4651460240487472</v>
       </c>
       <c r="G17">
-        <v>0.0536755355027598</v>
+        <v>1.382964078132105</v>
       </c>
       <c r="H17">
-        <v>-0.1821129130839084</v>
+        <v>0.01176848059693203</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -995,25 +1286,25 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.1476338940440795</v>
+        <v>1.104373464336496</v>
       </c>
       <c r="C18">
-        <v>-0.2489848374783721</v>
+        <v>2.756317658479167</v>
       </c>
       <c r="D18">
-        <v>0.005067197645347965</v>
+        <v>0.33622265652348</v>
       </c>
       <c r="E18">
-        <v>0.2251915875189206</v>
+        <v>0.2426824363760437</v>
       </c>
       <c r="F18">
-        <v>-0.0105968610677476</v>
+        <v>1.160500490459401</v>
       </c>
       <c r="G18">
-        <v>-0.1895696185385323</v>
+        <v>-0.2106951070757714</v>
       </c>
       <c r="H18">
-        <v>-0.2001301487978533</v>
+        <v>-0.2654538391348256</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1021,25 +1312,25 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>-0.0323979044984018</v>
+        <v>2.694057702950561</v>
       </c>
       <c r="C19">
-        <v>0.1877264853751708</v>
+        <v>0.2739627009948732</v>
       </c>
       <c r="D19">
-        <v>-0.04806196321149736</v>
+        <v>0.1804224808474368</v>
       </c>
       <c r="E19">
-        <v>-0.2270347206822821</v>
+        <v>1.098240534930794</v>
       </c>
       <c r="F19">
-        <v>-0.2375952509416031</v>
+        <v>-0.2729550626043783</v>
       </c>
       <c r="G19">
-        <v>-0.4453143610997332</v>
+        <v>-0.3277137946634324</v>
       </c>
       <c r="H19">
-        <v>-0.2281054616248284</v>
+        <v>0.2824462652976026</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1047,25 +1338,25 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>-0.06996447561954</v>
+        <v>-0.1162025284993027</v>
       </c>
       <c r="C20">
-        <v>-0.2489372330903247</v>
+        <v>-0.209742748646739</v>
       </c>
       <c r="D20">
-        <v>-0.2594977633496457</v>
+        <v>0.7080753054366183</v>
       </c>
       <c r="E20">
-        <v>-0.4672168735077758</v>
+        <v>-0.6631202920985542</v>
       </c>
       <c r="F20">
-        <v>-0.2500079740328711</v>
+        <v>-0.7178790241576083</v>
       </c>
       <c r="G20">
-        <v>0.05967819522519041</v>
+        <v>-0.1077189641965732</v>
       </c>
       <c r="H20">
-        <v>-0.09462593860681362</v>
+        <v>-0.1038714485161929</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1073,25 +1364,25 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>-0.1713918715036764</v>
+        <v>-0.3239783368717981</v>
       </c>
       <c r="C21">
-        <v>-0.3791109816618064</v>
+        <v>0.5938397172115593</v>
       </c>
       <c r="D21">
-        <v>-0.1619020821869017</v>
+        <v>-0.7773558803236132</v>
       </c>
       <c r="E21">
-        <v>0.1477840870711598</v>
+        <v>-0.8321146123826674</v>
       </c>
       <c r="F21">
-        <v>-0.006520046760844223</v>
+        <v>-0.2219545524216323</v>
       </c>
       <c r="G21">
-        <v>0.643906374458339</v>
+        <v>-0.218107036741252</v>
       </c>
       <c r="H21">
-        <v>0.4277413258401298</v>
+        <v>0.1864947913716819</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1099,25 +1390,25 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>-0.06818896562035748</v>
+        <v>0.3904210714055196</v>
       </c>
       <c r="C22">
-        <v>0.241497203637704</v>
+        <v>-0.980774526129653</v>
       </c>
       <c r="D22">
-        <v>0.08719306980569996</v>
+        <v>-1.035533258188707</v>
       </c>
       <c r="E22">
-        <v>0.7376194910248832</v>
+        <v>-0.425373198227672</v>
       </c>
       <c r="F22">
-        <v>0.521454442406674</v>
+        <v>-0.4215256825472917</v>
       </c>
       <c r="G22">
-        <v>0.1144253133717177</v>
+        <v>-0.01692385443435779</v>
       </c>
       <c r="H22">
-        <v>0.6134675305491375</v>
+        <v>-0.869687462795814</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1125,25 +1416,25 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.2497007499081394</v>
+        <v>-1.111494647333912</v>
       </c>
       <c r="C23">
-        <v>0.09539661607613537</v>
+        <v>-1.166253379392966</v>
       </c>
       <c r="D23">
-        <v>0.7458230372953185</v>
+        <v>-0.5560933194319311</v>
       </c>
       <c r="E23">
-        <v>0.5296579886771094</v>
+        <v>-0.5522458037515507</v>
       </c>
       <c r="F23">
-        <v>0.1226288596421531</v>
+        <v>-0.1476439756386168</v>
       </c>
       <c r="G23">
-        <v>0.6216710768195729</v>
+        <v>-1.000407584000073</v>
       </c>
       <c r="H23">
-        <v>0.4628221636640603</v>
+        <v>0.07930775132141864</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1151,25 +1442,25 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.09280705542466716</v>
+        <v>-0.9885452031585195</v>
       </c>
       <c r="C24">
-        <v>0.7432334766438504</v>
+        <v>-0.3783851431974844</v>
       </c>
       <c r="D24">
-        <v>0.5270684280256412</v>
+        <v>-0.3745376275171041</v>
       </c>
       <c r="E24">
-        <v>0.1200392989906849</v>
+        <v>0.03006420059582979</v>
       </c>
       <c r="F24">
-        <v>0.6190815161681047</v>
+        <v>-0.8226994077656263</v>
       </c>
       <c r="G24">
-        <v>0.4602326030125921</v>
+        <v>0.2570159275558653</v>
       </c>
       <c r="H24">
-        <v>0.5163964239828361</v>
+        <v>0.6520958313537208</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1177,25 +1468,25 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.7497668092269023</v>
+        <v>-0.342104639056839</v>
       </c>
       <c r="C25">
-        <v>0.5336017606086931</v>
+        <v>-0.3382571233764587</v>
       </c>
       <c r="D25">
-        <v>0.1265726315737368</v>
+        <v>0.06634470473647519</v>
       </c>
       <c r="E25">
-        <v>0.6256148487511566</v>
+        <v>-0.7864189036249809</v>
       </c>
       <c r="F25">
-        <v>0.466765935595644</v>
+        <v>0.2932964316965107</v>
       </c>
       <c r="G25">
-        <v>0.522929756565888</v>
+        <v>0.6883763354943663</v>
       </c>
       <c r="H25">
-        <v>2.77273259617728</v>
+        <v>0.6499866694232235</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1203,25 +1494,25 @@
         <v>31</v>
       </c>
       <c r="B26">
-        <v>0.4223850656296224</v>
+        <v>-0.4109081835817727</v>
       </c>
       <c r="C26">
-        <v>0.01535593659466611</v>
+        <v>-0.006306355468838787</v>
       </c>
       <c r="D26">
-        <v>0.5143981537720859</v>
+        <v>-0.859069963830295</v>
       </c>
       <c r="E26">
-        <v>0.3555492406165733</v>
+        <v>0.2206453714911967</v>
       </c>
       <c r="F26">
-        <v>0.4117130615868174</v>
+        <v>0.6157252752890523</v>
       </c>
       <c r="G26">
-        <v>2.661515901198209</v>
+        <v>0.5773356092179095</v>
       </c>
       <c r="H26">
-        <v>10.1306662320555</v>
+        <v>-1.277169042313017</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1229,25 +1520,25 @@
         <v>32</v>
       </c>
       <c r="B27">
-        <v>-0.02639020739223796</v>
+        <v>0.05964570376461731</v>
       </c>
       <c r="C27">
-        <v>0.4726520097851818</v>
+        <v>-0.7931179045968388</v>
       </c>
       <c r="D27">
-        <v>0.3138030966296693</v>
+        <v>0.2865974307246528</v>
       </c>
       <c r="E27">
-        <v>0.3699669175999133</v>
+        <v>0.6816773345225084</v>
       </c>
       <c r="F27">
-        <v>2.619769757211305</v>
+        <v>0.6432876684513655</v>
       </c>
       <c r="G27">
-        <v>10.0889200880686</v>
+        <v>-1.211216983079561</v>
       </c>
       <c r="H27">
-        <v>-8.082341712068869</v>
+        <v>-0.5362043056474258</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1255,25 +1546,25 @@
         <v>33</v>
       </c>
       <c r="B28">
-        <v>0.4979670725178967</v>
+        <v>-0.7566443719335638</v>
       </c>
       <c r="C28">
-        <v>0.3391181593623842</v>
+        <v>0.3230709633879277</v>
       </c>
       <c r="D28">
-        <v>0.3952819803326282</v>
+        <v>0.7181508671857834</v>
       </c>
       <c r="E28">
-        <v>2.64508481994402</v>
+        <v>0.6797612011146406</v>
       </c>
       <c r="F28">
-        <v>10.11423515080131</v>
+        <v>-1.174743450416286</v>
       </c>
       <c r="G28">
-        <v>-8.057026649336155</v>
+        <v>-0.4997307729841509</v>
       </c>
       <c r="H28">
-        <v>0.0826448976429941</v>
+        <v>0.2321195938041262</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1281,25 +1572,25 @@
         <v>34</v>
       </c>
       <c r="B29">
-        <v>0.343156824405298</v>
+        <v>0.4434691141957706</v>
       </c>
       <c r="C29">
-        <v>0.3993206453755421</v>
+        <v>0.8385490179936261</v>
       </c>
       <c r="D29">
-        <v>2.649123484986935</v>
+        <v>0.8001593519224834</v>
       </c>
       <c r="E29">
-        <v>10.11827381584423</v>
+        <v>-1.054345299608443</v>
       </c>
       <c r="F29">
-        <v>-8.052987984293241</v>
+        <v>-0.379332622176308</v>
       </c>
       <c r="G29">
-        <v>0.08668356268590799</v>
+        <v>0.3525177446119691</v>
       </c>
       <c r="H29">
-        <v>2.2342540344853</v>
+        <v>-0.01002219802129067</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1307,25 +1598,25 @@
         <v>35</v>
       </c>
       <c r="B30">
-        <v>0.2804435086845197</v>
+        <v>1.016170054683587</v>
       </c>
       <c r="C30">
-        <v>2.530246348295912</v>
+        <v>0.9777803886124443</v>
       </c>
       <c r="D30">
-        <v>9.999396679153206</v>
+        <v>-0.8767242629184823</v>
       </c>
       <c r="E30">
-        <v>-8.171865120984263</v>
+        <v>-0.2017115854863472</v>
       </c>
       <c r="F30">
-        <v>-0.03219357400511441</v>
+        <v>0.5301387813019299</v>
       </c>
       <c r="G30">
-        <v>2.115376897794278</v>
+        <v>0.1675988386686702</v>
       </c>
       <c r="H30">
-        <v>-1.324653088729052</v>
+        <v>-0.4025943082831233</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1333,25 +1624,25 @@
         <v>36</v>
       </c>
       <c r="B31">
-        <v>2.48932270964054</v>
+        <v>0.8910481548122668</v>
       </c>
       <c r="C31">
-        <v>9.958473040497832</v>
+        <v>-0.9634564967186597</v>
       </c>
       <c r="D31">
-        <v>-8.212788759639636</v>
+        <v>-0.2884438192865246</v>
       </c>
       <c r="E31">
-        <v>-0.07311721266048643</v>
+        <v>0.4434065475017525</v>
       </c>
       <c r="F31">
-        <v>2.074453259138906</v>
+        <v>0.08086660486849273</v>
       </c>
       <c r="G31">
-        <v>-1.365576727384424</v>
+        <v>-0.4893265420833007</v>
       </c>
       <c r="H31">
-        <v>-1.426750905798625</v>
+        <v>-0.2610848142822076</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1359,25 +1650,25 @@
         <v>37</v>
       </c>
       <c r="B32">
-        <v>9.643547872076862</v>
+        <v>-1.052940555106865</v>
       </c>
       <c r="C32">
-        <v>-8.527713928060606</v>
+        <v>-0.3779278776747304</v>
       </c>
       <c r="D32">
-        <v>-0.388042381081458</v>
+        <v>0.3539224891135467</v>
       </c>
       <c r="E32">
-        <v>1.759528090717934</v>
+        <v>-0.008617453519712992</v>
       </c>
       <c r="F32">
-        <v>-1.680501895805395</v>
+        <v>-0.5788106004715065</v>
       </c>
       <c r="G32">
-        <v>-1.741676074219596</v>
+        <v>-0.3505688726704134</v>
       </c>
       <c r="H32">
-        <v>0.2997798629366579</v>
+        <v>0.1514995940145626</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1385,25 +1676,25 @@
         <v>38</v>
       </c>
       <c r="B33">
-        <v>-9.584088888243137</v>
+        <v>-0.243604964186073</v>
       </c>
       <c r="C33">
-        <v>-1.444417341263988</v>
+        <v>0.4882454026022041</v>
       </c>
       <c r="D33">
-        <v>0.7031531305354048</v>
+        <v>0.1257054599689443</v>
       </c>
       <c r="E33">
-        <v>-2.736876855987925</v>
+        <v>-0.4444876869828491</v>
       </c>
       <c r="F33">
-        <v>-2.798051034402126</v>
+        <v>-0.216245959181756</v>
       </c>
       <c r="G33">
-        <v>-0.7565950972458717</v>
+        <v>0.2858225075032199</v>
       </c>
       <c r="H33">
-        <v>-1.339189634279513</v>
+        <v>-0.386254130202938</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1411,25 +1702,25 @@
         <v>39</v>
       </c>
       <c r="B34">
-        <v>-0.573770965293057</v>
+        <v>0.4515744274583506</v>
       </c>
       <c r="C34">
-        <v>1.573799506506335</v>
+        <v>0.08903448482509091</v>
       </c>
       <c r="D34">
-        <v>-1.866230480016994</v>
+        <v>-0.4811586621267026</v>
       </c>
       <c r="E34">
-        <v>-1.927404658431195</v>
+        <v>-0.2529169343256095</v>
       </c>
       <c r="F34">
-        <v>0.1140512787250589</v>
+        <v>0.2491515323593665</v>
       </c>
       <c r="G34">
-        <v>-0.4685432583085821</v>
+        <v>-0.4229251053467914</v>
       </c>
       <c r="H34">
-        <v>-0.3728682174992243</v>
+        <v>0.4285157694859537</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1437,25 +1728,25 @@
         <v>40</v>
       </c>
       <c r="B35">
-        <v>1.563148290176452</v>
+        <v>0.01105782720502824</v>
       </c>
       <c r="C35">
-        <v>-1.876881696346878</v>
+        <v>-0.5591353197467652</v>
       </c>
       <c r="D35">
-        <v>-1.938055874761079</v>
+        <v>-0.3308935919456721</v>
       </c>
       <c r="E35">
-        <v>0.1034000623951754</v>
+        <v>0.1711748747393038</v>
       </c>
       <c r="F35">
-        <v>-0.4791944746384656</v>
+        <v>-0.5009017629668541</v>
       </c>
       <c r="G35">
-        <v>-0.3835194338291078</v>
+        <v>0.350539111865891</v>
       </c>
       <c r="H35">
-        <v>-0.6439384708278306</v>
+        <v>-0.4178783160168349</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1463,25 +1754,25 @@
         <v>41</v>
       </c>
       <c r="B36">
-        <v>-1.985496228563019</v>
+        <v>-0.5719927198451231</v>
       </c>
       <c r="C36">
-        <v>-2.04667040697722</v>
+        <v>-0.34375099204403</v>
       </c>
       <c r="D36">
-        <v>-0.005214469820965406</v>
+        <v>0.1583174746409459</v>
       </c>
       <c r="E36">
-        <v>-0.5878090068546065</v>
+        <v>-0.513759163065212</v>
       </c>
       <c r="F36">
-        <v>-0.4921339660452486</v>
+        <v>0.3376817117675331</v>
       </c>
       <c r="G36">
-        <v>-0.7525530030439714</v>
+        <v>-0.4307357161151928</v>
       </c>
       <c r="H36">
-        <v>0.08290199311451979</v>
+        <v>0.8134071408387502</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1489,25 +1780,25 @@
         <v>42</v>
       </c>
       <c r="B37">
-        <v>-1.838568686009481</v>
+        <v>-0.368871833241708</v>
       </c>
       <c r="C37">
-        <v>0.2028872511467736</v>
+        <v>0.133196633443268</v>
       </c>
       <c r="D37">
-        <v>-0.3797072858868674</v>
+        <v>-0.5388800042628898</v>
       </c>
       <c r="E37">
-        <v>-0.2840322450775096</v>
+        <v>0.3125608705698552</v>
       </c>
       <c r="F37">
-        <v>-0.5444512820762324</v>
+        <v>-0.4558565573128707</v>
       </c>
       <c r="G37">
-        <v>0.2910037140822588</v>
+        <v>0.7882862996410722</v>
       </c>
       <c r="H37">
-        <v>0.1909243541796373</v>
+        <v>-0.02487289018377264</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1515,25 +1806,25 @@
         <v>43</v>
       </c>
       <c r="B38">
-        <v>0.319385421520574</v>
+        <v>0.1856282283015772</v>
       </c>
       <c r="C38">
-        <v>-0.263209115513067</v>
+        <v>-0.4864484094045807</v>
       </c>
       <c r="D38">
-        <v>-0.1675340747037092</v>
+        <v>0.3649924654281644</v>
       </c>
       <c r="E38">
-        <v>-0.427953111702432</v>
+        <v>-0.4034249624545615</v>
       </c>
       <c r="F38">
-        <v>0.4075018844560592</v>
+        <v>0.8407178944993815</v>
       </c>
       <c r="G38">
-        <v>0.3074225245534377</v>
+        <v>0.02755870467453658</v>
       </c>
       <c r="H38">
-        <v>-0.04636398152625851</v>
+        <v>0.4234297605040608</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1541,25 +1832,25 @@
         <v>44</v>
       </c>
       <c r="B39">
-        <v>-0.2177157015159319</v>
+        <v>-0.5341537593894865</v>
       </c>
       <c r="C39">
-        <v>-0.1220406607065741</v>
+        <v>0.3172871154432586</v>
       </c>
       <c r="D39">
-        <v>-0.3824596977052969</v>
+        <v>-0.4511303124394673</v>
       </c>
       <c r="E39">
-        <v>0.4529952984531944</v>
+        <v>0.7930125445144757</v>
       </c>
       <c r="F39">
-        <v>0.3529159385505728</v>
+        <v>-0.02014664531036925</v>
       </c>
       <c r="G39">
-        <v>-0.0008705675291234075</v>
+        <v>0.375724410519155</v>
       </c>
       <c r="H39">
-        <v>0.1473068229033219</v>
+        <v>-0.3002541768360317</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1567,25 +1858,25 @@
         <v>45</v>
       </c>
       <c r="B40">
-        <v>-0.1395947820665385</v>
+        <v>0.4376220803734752</v>
       </c>
       <c r="C40">
-        <v>-0.4000138190652613</v>
+        <v>-0.3307953475092508</v>
       </c>
       <c r="D40">
-        <v>0.4354411770932299</v>
+        <v>0.9133475094446922</v>
       </c>
       <c r="E40">
-        <v>0.3353618171906084</v>
+        <v>0.1001883196198473</v>
       </c>
       <c r="F40">
-        <v>-0.01842468888908786</v>
+        <v>0.4960593754493716</v>
       </c>
       <c r="G40">
-        <v>0.1297527015433575</v>
+        <v>-0.1799192119058152</v>
       </c>
       <c r="H40">
-        <v>0.2871986905475125</v>
+        <v>-0.1526582404267441</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1593,25 +1884,25 @@
         <v>46</v>
       </c>
       <c r="B41">
-        <v>-0.3119065001142551</v>
+        <v>-0.276523978776323</v>
       </c>
       <c r="C41">
-        <v>0.5235484960442361</v>
+        <v>0.96761887817762</v>
       </c>
       <c r="D41">
-        <v>0.4234691361416146</v>
+        <v>0.1544596883527751</v>
       </c>
       <c r="E41">
-        <v>0.06968263006191837</v>
+        <v>0.5503307441822993</v>
       </c>
       <c r="F41">
-        <v>0.2178600204943637</v>
+        <v>-0.1256478431728874</v>
       </c>
       <c r="G41">
-        <v>0.3753060094985187</v>
+        <v>-0.09838687169381632</v>
       </c>
       <c r="H41">
-        <v>-0.1253534470275521</v>
+        <v>-0.06690702153892325</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1619,25 +1910,25 @@
         <v>47</v>
       </c>
       <c r="B42">
-        <v>0.7021231295320197</v>
+        <v>1.045587057930149</v>
       </c>
       <c r="C42">
-        <v>0.6020437696293982</v>
+        <v>0.232427868105304</v>
       </c>
       <c r="D42">
-        <v>0.248257263549702</v>
+        <v>0.6282989239348282</v>
       </c>
       <c r="E42">
-        <v>0.3964346539821473</v>
+        <v>-0.04767966342035845</v>
       </c>
       <c r="F42">
-        <v>0.5538806429863024</v>
+        <v>-0.02041869194128743</v>
       </c>
       <c r="G42">
-        <v>0.0532211864602315</v>
+        <v>0.01106115821360565</v>
       </c>
       <c r="H42">
-        <v>0.3335790669957007</v>
+        <v>-0.4776050478021834</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1645,25 +1936,25 @@
         <v>48</v>
       </c>
       <c r="B43">
-        <v>1.514070997382048</v>
+        <v>0.05639396246521888</v>
       </c>
       <c r="C43">
-        <v>1.160284491302352</v>
+        <v>0.4522650182947431</v>
       </c>
       <c r="D43">
-        <v>1.308461881734797</v>
+        <v>-0.2237135690604436</v>
       </c>
       <c r="E43">
-        <v>1.465907870738952</v>
+        <v>-0.1964525975813726</v>
       </c>
       <c r="F43">
-        <v>0.9652484142128814</v>
+        <v>-0.1649727474264795</v>
       </c>
       <c r="G43">
-        <v>1.245606294748351</v>
+        <v>-0.6536389534422685</v>
       </c>
       <c r="H43">
-        <v>1.073631436903339</v>
+        <v>-0.07020966389325611</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1671,25 +1962,25 @@
         <v>49</v>
       </c>
       <c r="B44">
-        <v>0.2163102553365951</v>
+        <v>0.3510214679887943</v>
       </c>
       <c r="C44">
-        <v>0.3644876457690405</v>
+        <v>-0.3249571193663924</v>
       </c>
       <c r="D44">
-        <v>0.5219336347731955</v>
+        <v>-0.2976961478873214</v>
       </c>
       <c r="E44">
-        <v>0.02127417824712469</v>
+        <v>-0.2662162977324283</v>
       </c>
       <c r="F44">
-        <v>0.3016320587825939</v>
+        <v>-0.7548825037482174</v>
       </c>
       <c r="G44">
-        <v>0.1296572009375822</v>
+        <v>-0.171453214199205</v>
       </c>
       <c r="H44">
-        <v>0.4355197406839137</v>
+        <v>0.1863345695439667</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1697,25 +1988,25 @@
         <v>50</v>
       </c>
       <c r="B45">
-        <v>0.3684555432821496</v>
+        <v>-0.4071310593091498</v>
       </c>
       <c r="C45">
-        <v>0.5259015322863045</v>
+        <v>-0.3798700878300788</v>
       </c>
       <c r="D45">
-        <v>0.0252420757602338</v>
+        <v>-0.3483902376751857</v>
       </c>
       <c r="E45">
-        <v>0.305599956295703</v>
+        <v>-0.8370564436909746</v>
       </c>
       <c r="F45">
-        <v>0.1336250984506913</v>
+        <v>-0.2536271541419623</v>
       </c>
       <c r="G45">
-        <v>0.4394876381970228</v>
+        <v>0.1041606296012093</v>
       </c>
       <c r="H45">
-        <v>-0.1728423144902634</v>
+        <v>-0.05950864343986956</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1723,25 +2014,25 @@
         <v>51</v>
       </c>
       <c r="B46">
-        <v>0.661541622456546</v>
+        <v>-0.2355677475613481</v>
       </c>
       <c r="C46">
-        <v>0.1608821659304752</v>
+        <v>-0.204087897406455</v>
       </c>
       <c r="D46">
-        <v>0.4412400464659443</v>
+        <v>-0.692754103422244</v>
       </c>
       <c r="E46">
-        <v>0.2692651886209327</v>
+        <v>-0.1093248138732316</v>
       </c>
       <c r="F46">
-        <v>0.5751277283672642</v>
+        <v>0.24846296986994</v>
       </c>
       <c r="G46">
-        <v>-0.03720222432002201</v>
+        <v>0.08479369682886112</v>
       </c>
       <c r="H46">
-        <v>0.6511691608790895</v>
+        <v>0.4857584291303365</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1749,22 +2040,25 @@
         <v>52</v>
       </c>
       <c r="B47">
-        <v>-0.07992401592518952</v>
+        <v>-0.2348426952837251</v>
       </c>
       <c r="C47">
-        <v>0.2004338646102796</v>
+        <v>-0.7235089012995142</v>
       </c>
       <c r="D47">
-        <v>0.028459006765268</v>
+        <v>-0.1400796117505017</v>
       </c>
       <c r="E47">
-        <v>0.3343215465115995</v>
+        <v>0.2177081719926699</v>
       </c>
       <c r="F47">
-        <v>-0.2780084061756867</v>
+        <v>0.05403889895159103</v>
       </c>
       <c r="G47">
-        <v>0.4103629790234248</v>
+        <v>0.4550036312530664</v>
+      </c>
+      <c r="H47">
+        <v>0.5658775155607452</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1772,69 +2066,2567 @@
         <v>53</v>
       </c>
       <c r="B48">
-        <v>0.1551026493581833</v>
+        <v>-0.6900849287075143</v>
       </c>
       <c r="C48">
-        <v>-0.01687220848682837</v>
+        <v>-0.1066556391585018</v>
       </c>
       <c r="D48">
-        <v>0.2889903312595031</v>
+        <v>0.2511321445846698</v>
       </c>
       <c r="E48">
-        <v>-0.3233396214277831</v>
+        <v>0.08746287154359089</v>
       </c>
       <c r="F48">
-        <v>0.3650317637713285</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>0.4884276038450663</v>
+      </c>
+      <c r="G48">
+        <v>0.5993014881527451</v>
+      </c>
+      <c r="H48">
+        <v>0.7124381917287723</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B49">
-        <v>-0.08373363042288225</v>
+        <v>-0.03632087813986062</v>
       </c>
       <c r="C49">
-        <v>0.2221289093234493</v>
+        <v>0.321466905603311</v>
       </c>
       <c r="D49">
-        <v>-0.3902010433638369</v>
+        <v>0.1577976325622321</v>
       </c>
       <c r="E49">
-        <v>0.2981703418352746</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>0.5587623648637076</v>
+      </c>
+      <c r="F49">
+        <v>0.6696362491713863</v>
+      </c>
+      <c r="G49">
+        <v>0.7827729527474134</v>
+      </c>
+      <c r="H49">
+        <v>0.3586121302023135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B50">
-        <v>0.1925427069667326</v>
+        <v>0.2726965328743847</v>
       </c>
       <c r="C50">
-        <v>-0.4197872457205535</v>
+        <v>0.1090272598333058</v>
       </c>
       <c r="D50">
-        <v>0.268584139478558</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>0.5099919921347812</v>
+      </c>
+      <c r="E50">
+        <v>0.6208658764424599</v>
+      </c>
+      <c r="F50">
+        <v>0.7340025800184872</v>
+      </c>
+      <c r="G50">
+        <v>0.3098417574733872</v>
+      </c>
+      <c r="H50">
+        <v>0.2073791896271339</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B51">
-        <v>-0.4379379024501944</v>
+        <v>0.1665256447505902</v>
       </c>
       <c r="C51">
-        <v>0.2504334827489171</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>0.5674903770520656</v>
+      </c>
+      <c r="D51">
+        <v>0.6783642613597444</v>
+      </c>
+      <c r="E51">
+        <v>0.7915009649357716</v>
+      </c>
+      <c r="F51">
+        <v>0.3673401423906716</v>
+      </c>
+      <c r="G51">
+        <v>0.2648775745444182</v>
+      </c>
+      <c r="H51">
+        <v>0.2693183940473979</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B52">
+        <v>0.5748569778633511</v>
+      </c>
+      <c r="C52">
+        <v>0.6857308621710299</v>
+      </c>
+      <c r="D52">
+        <v>0.798867565747057</v>
+      </c>
+      <c r="E52">
+        <v>0.3747067432019571</v>
+      </c>
+      <c r="F52">
+        <v>0.2722441753557037</v>
+      </c>
+      <c r="G52">
+        <v>0.2766849948586834</v>
+      </c>
+      <c r="H52">
+        <v>0.5767620177460229</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53">
+        <v>0.7253260244454803</v>
+      </c>
+      <c r="C53">
+        <v>0.8384627280215076</v>
+      </c>
+      <c r="D53">
+        <v>0.4143019054764076</v>
+      </c>
+      <c r="E53">
+        <v>0.3118393376301542</v>
+      </c>
+      <c r="F53">
+        <v>0.3162801571331339</v>
+      </c>
+      <c r="G53">
+        <v>0.6163571800204733</v>
+      </c>
+      <c r="H53">
+        <v>0.8112287947142477</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54">
+        <v>0.7119811170863259</v>
+      </c>
+      <c r="C54">
+        <v>0.2878202945412259</v>
+      </c>
+      <c r="D54">
+        <v>0.1853577266949726</v>
+      </c>
+      <c r="E54">
+        <v>0.1897985461979523</v>
+      </c>
+      <c r="F54">
+        <v>0.4898755690852917</v>
+      </c>
+      <c r="G54">
+        <v>0.6847471837790661</v>
+      </c>
+      <c r="H54">
+        <v>0.5200616498372597</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55">
+        <v>0.287378348139204</v>
+      </c>
+      <c r="C55">
+        <v>0.1849157802929507</v>
+      </c>
+      <c r="D55">
+        <v>0.1893565997959304</v>
+      </c>
+      <c r="E55">
+        <v>0.4894336226832698</v>
+      </c>
+      <c r="F55">
+        <v>0.6843052373770442</v>
+      </c>
+      <c r="G55">
+        <v>0.5196197034352378</v>
+      </c>
+      <c r="H55">
+        <v>0.2378270114146924</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56">
+        <v>0.07636829124088795</v>
+      </c>
+      <c r="C56">
+        <v>0.08080911074386765</v>
+      </c>
+      <c r="D56">
+        <v>0.380886133631207</v>
+      </c>
+      <c r="E56">
+        <v>0.5757577483249815</v>
+      </c>
+      <c r="F56">
+        <v>0.411072214383175</v>
+      </c>
+      <c r="G56">
+        <v>0.1292795223626297</v>
+      </c>
+      <c r="H56">
+        <v>0.1337352025314798</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57">
+        <v>-0.01266405378425711</v>
+      </c>
+      <c r="C57">
+        <v>0.2874129691030823</v>
+      </c>
+      <c r="D57">
+        <v>0.4822845837968567</v>
+      </c>
+      <c r="E57">
+        <v>0.3175990498550503</v>
+      </c>
+      <c r="F57">
+        <v>0.03580635783450492</v>
+      </c>
+      <c r="G57">
+        <v>0.04026203800335501</v>
+      </c>
+      <c r="H57">
+        <v>-0.1837196931338607</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58">
+        <v>0.2282108395140873</v>
+      </c>
+      <c r="C58">
+        <v>0.4230824542078617</v>
+      </c>
+      <c r="D58">
+        <v>0.2583969202660553</v>
+      </c>
+      <c r="E58">
+        <v>-0.02339577175449009</v>
+      </c>
+      <c r="F58">
+        <v>-0.01894009158564</v>
+      </c>
+      <c r="G58">
+        <v>-0.2429218227228557</v>
+      </c>
+      <c r="H58">
+        <v>-0.2793693803839579</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59">
+        <v>0.3183656598562915</v>
+      </c>
+      <c r="C59">
+        <v>0.153680125914485</v>
+      </c>
+      <c r="D59">
+        <v>-0.1281125661060603</v>
+      </c>
+      <c r="E59">
+        <v>-0.1236568859372102</v>
+      </c>
+      <c r="F59">
+        <v>-0.3476386170744259</v>
+      </c>
+      <c r="G59">
+        <v>-0.3840861747355281</v>
+      </c>
+      <c r="H59">
+        <v>-0.008110489162830289</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60">
+        <v>0.126317124197464</v>
+      </c>
+      <c r="C60">
+        <v>-0.1554755678230814</v>
+      </c>
+      <c r="D60">
+        <v>-0.1510198876542313</v>
+      </c>
+      <c r="E60">
+        <v>-0.3750016187914469</v>
+      </c>
+      <c r="F60">
+        <v>-0.4114491764525492</v>
+      </c>
+      <c r="G60">
+        <v>-0.03547349087985135</v>
+      </c>
+      <c r="H60">
+        <v>0.296710085577183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61">
+        <v>-0.1461277552947611</v>
+      </c>
+      <c r="C61">
+        <v>-0.141672075125911</v>
+      </c>
+      <c r="D61">
+        <v>-0.3656538062631267</v>
+      </c>
+      <c r="E61">
+        <v>-0.4021013639242289</v>
+      </c>
+      <c r="F61">
+        <v>-0.02612567835153105</v>
+      </c>
+      <c r="G61">
+        <v>0.3060578981055033</v>
+      </c>
+      <c r="H61">
+        <v>-0.970759051217723</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62">
+        <v>-0.2150796810264732</v>
+      </c>
+      <c r="C62">
+        <v>-0.4390614121636889</v>
+      </c>
+      <c r="D62">
+        <v>-0.4755089698247911</v>
+      </c>
+      <c r="E62">
+        <v>-0.09953328425209329</v>
+      </c>
+      <c r="F62">
+        <v>0.2326502922049411</v>
+      </c>
+      <c r="G62">
+        <v>-1.044166657118285</v>
+      </c>
+      <c r="H62">
+        <v>-0.009761693010475867</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63">
+        <v>-0.4177648510533087</v>
+      </c>
+      <c r="C63">
+        <v>-0.454212408714411</v>
+      </c>
+      <c r="D63">
+        <v>-0.07823672314171318</v>
+      </c>
+      <c r="E63">
+        <v>0.2539468533153212</v>
+      </c>
+      <c r="F63">
+        <v>-1.022870096007905</v>
+      </c>
+      <c r="G63">
+        <v>0.01153486809990425</v>
+      </c>
+      <c r="H63">
+        <v>-0.5992195760667763</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64">
+        <v>-0.3908015821710129</v>
+      </c>
+      <c r="C64">
+        <v>-0.0148258965983151</v>
+      </c>
+      <c r="D64">
+        <v>0.3173576798587193</v>
+      </c>
+      <c r="E64">
+        <v>-0.959459269464507</v>
+      </c>
+      <c r="F64">
+        <v>0.07494569464330232</v>
+      </c>
+      <c r="G64">
+        <v>-0.5358087495233782</v>
+      </c>
+      <c r="H64">
+        <v>0.07502133209049482</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65">
+        <v>0.04051209196308692</v>
+      </c>
+      <c r="C65">
+        <v>0.3726956684201213</v>
+      </c>
+      <c r="D65">
+        <v>-0.904121280903105</v>
+      </c>
+      <c r="E65">
+        <v>0.1302836832047043</v>
+      </c>
+      <c r="F65">
+        <v>-0.4804707609619762</v>
+      </c>
+      <c r="G65">
+        <v>0.1303593206518968</v>
+      </c>
+      <c r="H65">
+        <v>-0.2253645994725027</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66">
+        <v>0.373022643048717</v>
+      </c>
+      <c r="C66">
+        <v>-0.9037943062745093</v>
+      </c>
+      <c r="D66">
+        <v>0.1306106578333001</v>
+      </c>
+      <c r="E66">
+        <v>-0.4801437863333805</v>
+      </c>
+      <c r="F66">
+        <v>0.1306862952804926</v>
+      </c>
+      <c r="G66">
+        <v>-0.225037624843907</v>
+      </c>
+      <c r="H66">
+        <v>-0.7607617588494426</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67">
+        <v>-0.9543715261257426</v>
+      </c>
+      <c r="C67">
+        <v>0.08003343798206668</v>
+      </c>
+      <c r="D67">
+        <v>-0.5307210061846139</v>
+      </c>
+      <c r="E67">
+        <v>0.08010907542925917</v>
+      </c>
+      <c r="F67">
+        <v>-0.2756148446951404</v>
+      </c>
+      <c r="G67">
+        <v>-0.811338978700676</v>
+      </c>
+      <c r="H67">
+        <v>-0.5449153543325702</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68">
+        <v>0.1567693963159068</v>
+      </c>
+      <c r="C68">
+        <v>-0.4539850478507738</v>
+      </c>
+      <c r="D68">
+        <v>0.1568450337630992</v>
+      </c>
+      <c r="E68">
+        <v>-0.1988788863613003</v>
+      </c>
+      <c r="F68">
+        <v>-0.7346030203668359</v>
+      </c>
+      <c r="G68">
+        <v>-0.4681793959987302</v>
+      </c>
+      <c r="H68">
+        <v>-0.7063590581727515</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69">
+        <v>-0.4809287046362252</v>
+      </c>
+      <c r="C69">
+        <v>0.1299013769776478</v>
+      </c>
+      <c r="D69">
+        <v>-0.2258225431467517</v>
+      </c>
+      <c r="E69">
+        <v>-0.7615466771522874</v>
+      </c>
+      <c r="F69">
+        <v>-0.4951230527841816</v>
+      </c>
+      <c r="G69">
+        <v>-0.733302714958203</v>
+      </c>
+      <c r="H69">
+        <v>-0.3711508662483193</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70">
+        <v>0.2566999892794087</v>
+      </c>
+      <c r="C70">
+        <v>-0.09902393084499078</v>
+      </c>
+      <c r="D70">
+        <v>-0.6347480648505264</v>
+      </c>
+      <c r="E70">
+        <v>-0.3683244404824207</v>
+      </c>
+      <c r="F70">
+        <v>-0.6065041026564419</v>
+      </c>
+      <c r="G70">
+        <v>-0.2443522539465584</v>
+      </c>
+      <c r="H70">
+        <v>0.007042287812221992</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71">
+        <v>-0.07257179750354642</v>
+      </c>
+      <c r="C71">
+        <v>-0.6082959315090821</v>
+      </c>
+      <c r="D71">
+        <v>-0.3418723071409763</v>
+      </c>
+      <c r="E71">
+        <v>-0.5800519693149977</v>
+      </c>
+      <c r="F71">
+        <v>-0.217900120605114</v>
+      </c>
+      <c r="G71">
+        <v>0.03349442115366635</v>
+      </c>
+      <c r="H71">
+        <v>-0.3906988058274866</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72">
+        <v>-0.5938449262677903</v>
+      </c>
+      <c r="C72">
+        <v>-0.3274213018996845</v>
+      </c>
+      <c r="D72">
+        <v>-0.5656009640737059</v>
+      </c>
+      <c r="E72">
+        <v>-0.2034491153638222</v>
+      </c>
+      <c r="F72">
+        <v>0.04794542639495819</v>
+      </c>
+      <c r="G72">
+        <v>-0.3762478005861947</v>
+      </c>
+      <c r="H72">
+        <v>0.0411736474925577</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73">
+        <v>-0.2914209188000479</v>
+      </c>
+      <c r="C73">
+        <v>-0.5296005809740691</v>
+      </c>
+      <c r="D73">
+        <v>-0.1674487322641856</v>
+      </c>
+      <c r="E73">
+        <v>0.08394580949459479</v>
+      </c>
+      <c r="F73">
+        <v>-0.3402474174865581</v>
+      </c>
+      <c r="G73">
+        <v>0.0771740305921943</v>
+      </c>
+      <c r="H73">
+        <v>-1.184815575379947</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74">
+        <v>-0.4748093065875613</v>
+      </c>
+      <c r="C74">
+        <v>-0.1126574578776777</v>
+      </c>
+      <c r="D74">
+        <v>0.1387370838811027</v>
+      </c>
+      <c r="E74">
+        <v>-0.2854561431000502</v>
+      </c>
+      <c r="F74">
+        <v>0.1319653049787022</v>
+      </c>
+      <c r="G74">
+        <v>-1.130024300993439</v>
+      </c>
+      <c r="H74">
+        <v>0.8937838266029242</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75">
+        <v>0.01478900777879333</v>
+      </c>
+      <c r="C75">
+        <v>0.2661835495375737</v>
+      </c>
+      <c r="D75">
+        <v>-0.1580096774435792</v>
+      </c>
+      <c r="E75">
+        <v>0.2594117706351732</v>
+      </c>
+      <c r="F75">
+        <v>-1.002577835336968</v>
+      </c>
+      <c r="G75">
+        <v>1.021230292259395</v>
+      </c>
+      <c r="H75">
+        <v>1.049879113070932</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76">
+        <v>0.3526062080970701</v>
+      </c>
+      <c r="C76">
+        <v>-0.07158701888408281</v>
+      </c>
+      <c r="D76">
+        <v>0.3458344291946696</v>
+      </c>
+      <c r="E76">
+        <v>-0.9161551767774719</v>
+      </c>
+      <c r="F76">
+        <v>1.107652950818892</v>
+      </c>
+      <c r="G76">
+        <v>1.136301771630429</v>
+      </c>
+      <c r="H76">
+        <v>2.719830598090047</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77">
+        <v>-0.05399120883067776</v>
+      </c>
+      <c r="C77">
+        <v>0.3634302392480747</v>
+      </c>
+      <c r="D77">
+        <v>-0.8985593667240669</v>
+      </c>
+      <c r="E77">
+        <v>1.125248760872297</v>
+      </c>
+      <c r="F77">
+        <v>1.153897581683834</v>
+      </c>
+      <c r="G77">
+        <v>2.737426408143452</v>
+      </c>
+      <c r="H77">
+        <v>4.430247296085167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78">
+        <v>0.3963761775604042</v>
+      </c>
+      <c r="C78">
+        <v>-0.8656134284117374</v>
+      </c>
+      <c r="D78">
+        <v>1.158194699184626</v>
+      </c>
+      <c r="E78">
+        <v>1.186843519996163</v>
+      </c>
+      <c r="F78">
+        <v>2.770372346455781</v>
+      </c>
+      <c r="G78">
+        <v>4.463193234397496</v>
+      </c>
+      <c r="H78">
+        <v>0.3449098147915402</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79">
+        <v>-0.8800736289835152</v>
+      </c>
+      <c r="C79">
+        <v>1.143734498612848</v>
+      </c>
+      <c r="D79">
+        <v>1.172383319424386</v>
+      </c>
+      <c r="E79">
+        <v>2.755912145884004</v>
+      </c>
+      <c r="F79">
+        <v>4.448733033825719</v>
+      </c>
+      <c r="G79">
+        <v>0.3304496142197624</v>
+      </c>
+      <c r="H79">
+        <v>-0.08006806134328093</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80">
+        <v>1.239931507228801</v>
+      </c>
+      <c r="C80">
+        <v>1.268580328040338</v>
+      </c>
+      <c r="D80">
+        <v>2.852109154499956</v>
+      </c>
+      <c r="E80">
+        <v>4.544930042441671</v>
+      </c>
+      <c r="F80">
+        <v>0.4266466228357149</v>
+      </c>
+      <c r="G80">
+        <v>0.01612894727267156</v>
+      </c>
+      <c r="H80">
+        <v>0.7346596165289111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81">
+        <v>1.179202422334401</v>
+      </c>
+      <c r="C81">
+        <v>2.762731248794019</v>
+      </c>
+      <c r="D81">
+        <v>4.455552136735734</v>
+      </c>
+      <c r="E81">
+        <v>0.3372687171297775</v>
+      </c>
+      <c r="F81">
+        <v>-0.07324895843326584</v>
+      </c>
+      <c r="G81">
+        <v>0.6452817108229737</v>
+      </c>
+      <c r="H81">
+        <v>0.4934385692022478</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82">
+        <v>2.646269414624167</v>
+      </c>
+      <c r="C82">
+        <v>4.339090302565882</v>
+      </c>
+      <c r="D82">
+        <v>0.2208068829599255</v>
+      </c>
+      <c r="E82">
+        <v>-0.1897107926031179</v>
+      </c>
+      <c r="F82">
+        <v>0.5288198766531217</v>
+      </c>
+      <c r="G82">
+        <v>0.3769767350323958</v>
+      </c>
+      <c r="H82">
+        <v>-1.643763506744272</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83">
+        <v>3.982591770669121</v>
+      </c>
+      <c r="C83">
+        <v>-0.135691648936835</v>
+      </c>
+      <c r="D83">
+        <v>-0.5462093244998784</v>
+      </c>
+      <c r="E83">
+        <v>0.1723213447563612</v>
+      </c>
+      <c r="F83">
+        <v>0.02047820313563531</v>
+      </c>
+      <c r="G83">
+        <v>-2.000262038641033</v>
+      </c>
+      <c r="H83">
+        <v>-0.5161864048812744</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84">
+        <v>-0.5974898394390895</v>
+      </c>
+      <c r="C84">
+        <v>-1.008007515002133</v>
+      </c>
+      <c r="D84">
+        <v>-0.2894768457458933</v>
+      </c>
+      <c r="E84">
+        <v>-0.4413199873666193</v>
+      </c>
+      <c r="F84">
+        <v>-2.462060229143287</v>
+      </c>
+      <c r="G84">
+        <v>-0.977984595383529</v>
+      </c>
+      <c r="H84">
+        <v>-0.6447655124219993</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85">
+        <v>-1.065388266313746</v>
+      </c>
+      <c r="C85">
+        <v>-0.3468575970575067</v>
+      </c>
+      <c r="D85">
+        <v>-0.4987007386782327</v>
+      </c>
+      <c r="E85">
+        <v>-2.519440980454901</v>
+      </c>
+      <c r="F85">
+        <v>-1.035365346695142</v>
+      </c>
+      <c r="G85">
+        <v>-0.7021462637336128</v>
+      </c>
+      <c r="H85">
+        <v>-1.836531446329783</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86">
+        <v>-0.2939646841069006</v>
+      </c>
+      <c r="C86">
+        <v>-0.4458078257276266</v>
+      </c>
+      <c r="D86">
+        <v>-2.466548067504295</v>
+      </c>
+      <c r="E86">
+        <v>-0.9824724337445363</v>
+      </c>
+      <c r="F86">
+        <v>-0.6492533507830067</v>
+      </c>
+      <c r="G86">
+        <v>-1.783638533379176</v>
+      </c>
+      <c r="H86">
+        <v>-0.4036785729014095</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87">
+        <v>-0.4753377773606906</v>
+      </c>
+      <c r="C87">
+        <v>-2.496078019137359</v>
+      </c>
+      <c r="D87">
+        <v>-1.0120023853776</v>
+      </c>
+      <c r="E87">
+        <v>-0.6787833024160707</v>
+      </c>
+      <c r="F87">
+        <v>-1.81316848501224</v>
+      </c>
+      <c r="G87">
+        <v>-0.4332085245344734</v>
+      </c>
+      <c r="H87">
+        <v>-0.8170043294446403</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88">
+        <v>-2.542893978309402</v>
+      </c>
+      <c r="C88">
+        <v>-1.058818344549643</v>
+      </c>
+      <c r="D88">
+        <v>-0.7255992615881137</v>
+      </c>
+      <c r="E88">
+        <v>-1.859984444184283</v>
+      </c>
+      <c r="F88">
+        <v>-0.4800244837065165</v>
+      </c>
+      <c r="G88">
+        <v>-0.8638202886166834</v>
+      </c>
+      <c r="H88">
+        <v>-0.1789343978423749</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B89">
+        <v>-0.8243033945289489</v>
+      </c>
+      <c r="C89">
+        <v>-0.4910843115674192</v>
+      </c>
+      <c r="D89">
+        <v>-1.625469494163589</v>
+      </c>
+      <c r="E89">
+        <v>-0.245509533685822</v>
+      </c>
+      <c r="F89">
+        <v>-0.6293053385959889</v>
+      </c>
+      <c r="G89">
+        <v>0.05558055217831959</v>
+      </c>
+      <c r="H89">
+        <v>-0.6364448322033516</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90">
+        <v>-0.5351204465965399</v>
+      </c>
+      <c r="C90">
+        <v>-1.66950562919271</v>
+      </c>
+      <c r="D90">
+        <v>-0.2895456687149427</v>
+      </c>
+      <c r="E90">
+        <v>-0.6733414736251095</v>
+      </c>
+      <c r="F90">
+        <v>0.0115444171491989</v>
+      </c>
+      <c r="G90">
+        <v>-0.6804809672324722</v>
+      </c>
+      <c r="H90">
+        <v>-0.4410326232298434</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91">
+        <v>-1.564154328600046</v>
+      </c>
+      <c r="C91">
+        <v>-0.1841943681222787</v>
+      </c>
+      <c r="D91">
+        <v>-0.5679901730324456</v>
+      </c>
+      <c r="E91">
+        <v>0.1168957177418629</v>
+      </c>
+      <c r="F91">
+        <v>-0.5751296666398082</v>
+      </c>
+      <c r="G91">
+        <v>-0.3356813226371794</v>
+      </c>
+      <c r="H91">
+        <v>-0.2989533458780087</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92">
+        <v>0.01136921538350649</v>
+      </c>
+      <c r="C92">
+        <v>-0.3724265895266604</v>
+      </c>
+      <c r="D92">
+        <v>0.3124593012476481</v>
+      </c>
+      <c r="E92">
+        <v>-0.3795660831340231</v>
+      </c>
+      <c r="F92">
+        <v>-0.1401177391313942</v>
+      </c>
+      <c r="G92">
+        <v>-0.1033897623722235</v>
+      </c>
+      <c r="H92">
+        <v>0.723104312015092</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B93">
+        <v>-0.1989446793676382</v>
+      </c>
+      <c r="C93">
+        <v>0.4859412114066703</v>
+      </c>
+      <c r="D93">
+        <v>-0.2060841729750008</v>
+      </c>
+      <c r="E93">
+        <v>0.03336417102762801</v>
+      </c>
+      <c r="F93">
+        <v>0.07009214778679873</v>
+      </c>
+      <c r="G93">
+        <v>0.8965862221741142</v>
+      </c>
+      <c r="H93">
+        <v>0.240788012052549</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94">
+        <v>0.9526635850093691</v>
+      </c>
+      <c r="C94">
+        <v>0.2606382006276979</v>
+      </c>
+      <c r="D94">
+        <v>0.5000865446303268</v>
+      </c>
+      <c r="E94">
+        <v>0.5368145213894975</v>
+      </c>
+      <c r="F94">
+        <v>1.363308595776813</v>
+      </c>
+      <c r="G94">
+        <v>0.7075103856552477</v>
+      </c>
+      <c r="H94">
+        <v>0.0493601459296269</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95">
+        <v>0.2183276878862375</v>
+      </c>
+      <c r="C95">
+        <v>0.4577760318888663</v>
+      </c>
+      <c r="D95">
+        <v>0.494504008648037</v>
+      </c>
+      <c r="E95">
+        <v>1.320998083035352</v>
+      </c>
+      <c r="F95">
+        <v>0.6651998729137872</v>
+      </c>
+      <c r="G95">
+        <v>0.007049633188166426</v>
+      </c>
+      <c r="H95">
+        <v>0.4061645810399495</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96">
+        <v>0.4274989419678774</v>
+      </c>
+      <c r="C96">
+        <v>0.4642269187270481</v>
+      </c>
+      <c r="D96">
+        <v>1.290720993114364</v>
+      </c>
+      <c r="E96">
+        <v>0.6349227829927984</v>
+      </c>
+      <c r="F96">
+        <v>-0.02322745673282245</v>
+      </c>
+      <c r="G96">
+        <v>0.3758874911189606</v>
+      </c>
+      <c r="H96">
+        <v>0.3144509489973832</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B97">
+        <v>0.451611734653072</v>
+      </c>
+      <c r="C97">
+        <v>1.278105809040388</v>
+      </c>
+      <c r="D97">
+        <v>0.6223075989188223</v>
+      </c>
+      <c r="E97">
+        <v>-0.03584264080679855</v>
+      </c>
+      <c r="F97">
+        <v>0.3632723070449845</v>
+      </c>
+      <c r="G97">
+        <v>0.3018357649234071</v>
+      </c>
+      <c r="H97">
+        <v>-0.1323301701936964</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B98">
+        <v>1.235029948750828</v>
+      </c>
+      <c r="C98">
+        <v>0.5792317386292632</v>
+      </c>
+      <c r="D98">
+        <v>-0.07891850109635756</v>
+      </c>
+      <c r="E98">
+        <v>0.3201964467554255</v>
+      </c>
+      <c r="F98">
+        <v>0.2587599046338481</v>
+      </c>
+      <c r="G98">
+        <v>-0.1754060304832554</v>
+      </c>
+      <c r="H98">
+        <v>0.8033953615958215</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B99">
+        <v>0.299808989306214</v>
+      </c>
+      <c r="C99">
+        <v>-0.3583412504194069</v>
+      </c>
+      <c r="D99">
+        <v>0.04077369743237619</v>
+      </c>
+      <c r="E99">
+        <v>-0.02066284468920121</v>
+      </c>
+      <c r="F99">
+        <v>-0.4548287798063048</v>
+      </c>
+      <c r="G99">
+        <v>0.5239726122727721</v>
+      </c>
+      <c r="H99">
+        <v>0.296856707824846</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B100">
+        <v>-0.4329776612703231</v>
+      </c>
+      <c r="C100">
+        <v>-0.03386271341853997</v>
+      </c>
+      <c r="D100">
+        <v>-0.09529925554011737</v>
+      </c>
+      <c r="E100">
+        <v>-0.529465190657221</v>
+      </c>
+      <c r="F100">
+        <v>0.449336201421856</v>
+      </c>
+      <c r="G100">
+        <v>0.2222202969739298</v>
+      </c>
+      <c r="H100">
+        <v>-0.4112394324521587</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101">
+        <v>-0.00299340778301399</v>
+      </c>
+      <c r="C101">
+        <v>-0.06442994990459139</v>
+      </c>
+      <c r="D101">
+        <v>-0.4985958850216949</v>
+      </c>
+      <c r="E101">
+        <v>0.480205507057382</v>
+      </c>
+      <c r="F101">
+        <v>0.2530896026094558</v>
+      </c>
+      <c r="G101">
+        <v>-0.3803701268166327</v>
+      </c>
+      <c r="H101">
+        <v>0.04702683183897161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102">
+        <v>-0.1856174723396913</v>
+      </c>
+      <c r="C102">
+        <v>-0.6197834074567948</v>
+      </c>
+      <c r="D102">
+        <v>0.3590179846222821</v>
+      </c>
+      <c r="E102">
+        <v>0.1319020801743559</v>
+      </c>
+      <c r="F102">
+        <v>-0.5015576492517326</v>
+      </c>
+      <c r="G102">
+        <v>-0.07416069059612829</v>
+      </c>
+      <c r="H102">
+        <v>-0.2404976452842752</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B103">
+        <v>-0.5905101764174595</v>
+      </c>
+      <c r="C103">
+        <v>0.3882912156616174</v>
+      </c>
+      <c r="D103">
+        <v>0.1611753112136912</v>
+      </c>
+      <c r="E103">
+        <v>-0.4722844182123973</v>
+      </c>
+      <c r="F103">
+        <v>-0.04488745955679299</v>
+      </c>
+      <c r="G103">
+        <v>-0.2112244142449399</v>
+      </c>
+      <c r="H103">
+        <v>-0.08851339780411407</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B104">
+        <v>0.4273407187267424</v>
+      </c>
+      <c r="C104">
+        <v>0.2002248142788162</v>
+      </c>
+      <c r="D104">
+        <v>-0.4332349151472724</v>
+      </c>
+      <c r="E104">
+        <v>-0.005837956491668017</v>
+      </c>
+      <c r="F104">
+        <v>-0.1721749111798149</v>
+      </c>
+      <c r="G104">
+        <v>-0.0494638947389891</v>
+      </c>
+      <c r="H104">
+        <v>-0.002230158183848807</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B105">
+        <v>0.1086983409703039</v>
+      </c>
+      <c r="C105">
+        <v>-0.5247613884557847</v>
+      </c>
+      <c r="D105">
+        <v>-0.09736442980018029</v>
+      </c>
+      <c r="E105">
+        <v>-0.2637013844883272</v>
+      </c>
+      <c r="F105">
+        <v>-0.1409903680475014</v>
+      </c>
+      <c r="G105">
+        <v>-0.09375663149236108</v>
+      </c>
+      <c r="H105">
+        <v>-0.4903753630148127</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B106">
+        <v>-0.5318964931771777</v>
+      </c>
+      <c r="C106">
+        <v>-0.1044995345215733</v>
+      </c>
+      <c r="D106">
+        <v>-0.2708364892097202</v>
+      </c>
+      <c r="E106">
+        <v>-0.1481254727688944</v>
+      </c>
+      <c r="F106">
+        <v>-0.1008917362137541</v>
+      </c>
+      <c r="G106">
+        <v>-0.4975104677362057</v>
+      </c>
+      <c r="H106">
+        <v>-0.2434584326124856</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B107">
+        <v>-0.04607696087735</v>
+      </c>
+      <c r="C107">
+        <v>-0.2124139155654969</v>
+      </c>
+      <c r="D107">
+        <v>-0.08970289912467108</v>
+      </c>
+      <c r="E107">
+        <v>-0.04246916256953079</v>
+      </c>
+      <c r="F107">
+        <v>-0.4390878940919825</v>
+      </c>
+      <c r="G107">
+        <v>-0.1850358589682623</v>
+      </c>
+      <c r="H107">
+        <v>0.03508853090531031</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B108">
+        <v>-0.1938269109680474</v>
+      </c>
+      <c r="C108">
+        <v>-0.07111589452722158</v>
+      </c>
+      <c r="D108">
+        <v>-0.02388215797208129</v>
+      </c>
+      <c r="E108">
+        <v>-0.4205008894945329</v>
+      </c>
+      <c r="F108">
+        <v>-0.1664488543708128</v>
+      </c>
+      <c r="G108">
+        <v>0.0536755355027598</v>
+      </c>
+      <c r="H108">
+        <v>-0.1821129130839084</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109">
+        <v>0.04184555234415971</v>
+      </c>
+      <c r="C109">
+        <v>0.0890792888993</v>
+      </c>
+      <c r="D109">
+        <v>-0.3075394426231516</v>
+      </c>
+      <c r="E109">
+        <v>-0.05348740749943154</v>
+      </c>
+      <c r="F109">
+        <v>0.1666369823741411</v>
+      </c>
+      <c r="G109">
+        <v>-0.0691514662125271</v>
+      </c>
+      <c r="H109">
+        <v>-0.2481242236833118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110">
+        <v>0.1476338940440795</v>
+      </c>
+      <c r="C110">
+        <v>-0.2489848374783721</v>
+      </c>
+      <c r="D110">
+        <v>0.005067197645347965</v>
+      </c>
+      <c r="E110">
+        <v>0.2251915875189206</v>
+      </c>
+      <c r="F110">
+        <v>-0.0105968610677476</v>
+      </c>
+      <c r="G110">
+        <v>-0.1895696185385323</v>
+      </c>
+      <c r="H110">
+        <v>-0.2001301487978533</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111">
+        <v>-0.31566407673435</v>
+      </c>
+      <c r="C111">
+        <v>-0.06161204161062994</v>
+      </c>
+      <c r="D111">
+        <v>0.1585123482629427</v>
+      </c>
+      <c r="E111">
+        <v>-0.07727610032372551</v>
+      </c>
+      <c r="F111">
+        <v>-0.2562488577945102</v>
+      </c>
+      <c r="G111">
+        <v>-0.2668093880538313</v>
+      </c>
+      <c r="H111">
+        <v>-0.4745284982119613</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B112">
+        <v>-0.0323979044984018</v>
+      </c>
+      <c r="C112">
+        <v>0.1877264853751708</v>
+      </c>
+      <c r="D112">
+        <v>-0.04806196321149736</v>
+      </c>
+      <c r="E112">
+        <v>-0.2270347206822821</v>
+      </c>
+      <c r="F112">
+        <v>-0.2375952509416031</v>
+      </c>
+      <c r="G112">
+        <v>-0.4453143610997332</v>
+      </c>
+      <c r="H112">
+        <v>-0.2281054616248284</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B113">
+        <v>0.2063695661061287</v>
+      </c>
+      <c r="C113">
+        <v>-0.02941888248053948</v>
+      </c>
+      <c r="D113">
+        <v>-0.2083916399513242</v>
+      </c>
+      <c r="E113">
+        <v>-0.2189521702106452</v>
+      </c>
+      <c r="F113">
+        <v>-0.4266712803687753</v>
+      </c>
+      <c r="G113">
+        <v>-0.2094623808938705</v>
+      </c>
+      <c r="H113">
+        <v>0.1002237883641909</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B114">
+        <v>-0.06996447561954</v>
+      </c>
+      <c r="C114">
+        <v>-0.2489372330903247</v>
+      </c>
+      <c r="D114">
+        <v>-0.2594977633496457</v>
+      </c>
+      <c r="E114">
+        <v>-0.4672168735077758</v>
+      </c>
+      <c r="F114">
+        <v>-0.2500079740328711</v>
+      </c>
+      <c r="G114">
+        <v>0.05967819522519041</v>
+      </c>
+      <c r="H114">
+        <v>-0.09462593860681362</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B115">
+        <v>-0.1949601066790565</v>
+      </c>
+      <c r="C115">
+        <v>-0.2055206369383775</v>
+      </c>
+      <c r="D115">
+        <v>-0.4132397470965076</v>
+      </c>
+      <c r="E115">
+        <v>-0.1960308476216028</v>
+      </c>
+      <c r="F115">
+        <v>0.1136553216364586</v>
+      </c>
+      <c r="G115">
+        <v>-0.04064881219554539</v>
+      </c>
+      <c r="H115">
+        <v>0.6097776090236378</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B116">
+        <v>-0.1713918715036764</v>
+      </c>
+      <c r="C116">
+        <v>-0.3791109816618064</v>
+      </c>
+      <c r="D116">
+        <v>-0.1619020821869017</v>
+      </c>
+      <c r="E116">
+        <v>0.1477840870711598</v>
+      </c>
+      <c r="F116">
+        <v>-0.006520046760844223</v>
+      </c>
+      <c r="G116">
+        <v>0.643906374458339</v>
+      </c>
+      <c r="H116">
+        <v>0.4277413258401298</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B117">
+        <v>-0.3763423975016759</v>
+      </c>
+      <c r="C117">
+        <v>-0.1591334980267711</v>
+      </c>
+      <c r="D117">
+        <v>0.1505526712312903</v>
+      </c>
+      <c r="E117">
+        <v>-0.003751462600713684</v>
+      </c>
+      <c r="F117">
+        <v>0.6466749586184695</v>
+      </c>
+      <c r="G117">
+        <v>0.4305099100002604</v>
+      </c>
+      <c r="H117">
+        <v>0.02348078096530404</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B118">
+        <v>-0.06818896562035748</v>
+      </c>
+      <c r="C118">
+        <v>0.241497203637704</v>
+      </c>
+      <c r="D118">
+        <v>0.08719306980569996</v>
+      </c>
+      <c r="E118">
+        <v>0.7376194910248832</v>
+      </c>
+      <c r="F118">
+        <v>0.521454442406674</v>
+      </c>
+      <c r="G118">
+        <v>0.1144253133717177</v>
+      </c>
+      <c r="H118">
+        <v>0.6134675305491375</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B119">
+        <v>0.2497007499081394</v>
+      </c>
+      <c r="C119">
+        <v>0.09539661607613537</v>
+      </c>
+      <c r="D119">
+        <v>0.7458230372953185</v>
+      </c>
+      <c r="E119">
+        <v>0.5296579886771094</v>
+      </c>
+      <c r="F119">
+        <v>0.1226288596421531</v>
+      </c>
+      <c r="G119">
+        <v>0.6216710768195729</v>
+      </c>
+      <c r="H119">
+        <v>0.4628221636640603</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B120">
+        <v>0.09280705542466716</v>
+      </c>
+      <c r="C120">
+        <v>0.7432334766438504</v>
+      </c>
+      <c r="D120">
+        <v>0.5270684280256412</v>
+      </c>
+      <c r="E120">
+        <v>0.1200392989906849</v>
+      </c>
+      <c r="F120">
+        <v>0.6190815161681047</v>
+      </c>
+      <c r="G120">
+        <v>0.4602326030125921</v>
+      </c>
+      <c r="H120">
+        <v>0.5163964239828361</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B121">
+        <v>0.7497668092269023</v>
+      </c>
+      <c r="C121">
+        <v>0.5336017606086931</v>
+      </c>
+      <c r="D121">
+        <v>0.1265726315737368</v>
+      </c>
+      <c r="E121">
+        <v>0.6256148487511566</v>
+      </c>
+      <c r="F121">
+        <v>0.466765935595644</v>
+      </c>
+      <c r="G121">
+        <v>0.522929756565888</v>
+      </c>
+      <c r="H121">
+        <v>2.77273259617728</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B122">
+        <v>0.4223850656296224</v>
+      </c>
+      <c r="C122">
+        <v>0.01535593659466611</v>
+      </c>
+      <c r="D122">
+        <v>0.5143981537720859</v>
+      </c>
+      <c r="E122">
+        <v>0.3555492406165733</v>
+      </c>
+      <c r="F122">
+        <v>0.4117130615868174</v>
+      </c>
+      <c r="G122">
+        <v>2.661515901198209</v>
+      </c>
+      <c r="H122">
+        <v>10.1306662320555</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B123">
+        <v>-0.02639020739223796</v>
+      </c>
+      <c r="C123">
+        <v>0.4726520097851818</v>
+      </c>
+      <c r="D123">
+        <v>0.3138030966296693</v>
+      </c>
+      <c r="E123">
+        <v>0.3699669175999133</v>
+      </c>
+      <c r="F123">
+        <v>2.619769757211305</v>
+      </c>
+      <c r="G123">
+        <v>10.0889200880686</v>
+      </c>
+      <c r="H123">
+        <v>-8.082341712068869</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B124">
+        <v>0.4979670725178967</v>
+      </c>
+      <c r="C124">
+        <v>0.3391181593623842</v>
+      </c>
+      <c r="D124">
+        <v>0.3952819803326282</v>
+      </c>
+      <c r="E124">
+        <v>2.64508481994402</v>
+      </c>
+      <c r="F124">
+        <v>10.11423515080131</v>
+      </c>
+      <c r="G124">
+        <v>-8.057026649336155</v>
+      </c>
+      <c r="H124">
+        <v>0.0826448976429941</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B125">
+        <v>0.343156824405298</v>
+      </c>
+      <c r="C125">
+        <v>0.3993206453755421</v>
+      </c>
+      <c r="D125">
+        <v>2.649123484986935</v>
+      </c>
+      <c r="E125">
+        <v>10.11827381584423</v>
+      </c>
+      <c r="F125">
+        <v>-8.052987984293241</v>
+      </c>
+      <c r="G125">
+        <v>0.08668356268590799</v>
+      </c>
+      <c r="H125">
+        <v>2.2342540344853</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B126">
+        <v>0.2804435086845197</v>
+      </c>
+      <c r="C126">
+        <v>2.530246348295912</v>
+      </c>
+      <c r="D126">
+        <v>9.999396679153206</v>
+      </c>
+      <c r="E126">
+        <v>-8.171865120984263</v>
+      </c>
+      <c r="F126">
+        <v>-0.03219357400511441</v>
+      </c>
+      <c r="G126">
+        <v>2.115376897794278</v>
+      </c>
+      <c r="H126">
+        <v>-1.324653088729052</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B127">
+        <v>2.48932270964054</v>
+      </c>
+      <c r="C127">
+        <v>9.958473040497832</v>
+      </c>
+      <c r="D127">
+        <v>-8.212788759639636</v>
+      </c>
+      <c r="E127">
+        <v>-0.07311721266048643</v>
+      </c>
+      <c r="F127">
+        <v>2.074453259138906</v>
+      </c>
+      <c r="G127">
+        <v>-1.365576727384424</v>
+      </c>
+      <c r="H127">
+        <v>-1.426750905798625</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B128">
+        <v>9.643547872076862</v>
+      </c>
+      <c r="C128">
+        <v>-8.527713928060606</v>
+      </c>
+      <c r="D128">
+        <v>-0.388042381081458</v>
+      </c>
+      <c r="E128">
+        <v>1.759528090717934</v>
+      </c>
+      <c r="F128">
+        <v>-1.680501895805395</v>
+      </c>
+      <c r="G128">
+        <v>-1.741676074219596</v>
+      </c>
+      <c r="H128">
+        <v>0.2997798629366579</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B129">
+        <v>-9.584088888243137</v>
+      </c>
+      <c r="C129">
+        <v>-1.444417341263988</v>
+      </c>
+      <c r="D129">
+        <v>0.7031531305354048</v>
+      </c>
+      <c r="E129">
+        <v>-2.736876855987925</v>
+      </c>
+      <c r="F129">
+        <v>-2.798051034402126</v>
+      </c>
+      <c r="G129">
+        <v>-0.7565950972458717</v>
+      </c>
+      <c r="H129">
+        <v>-1.339189634279513</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B130">
+        <v>-0.573770965293057</v>
+      </c>
+      <c r="C130">
+        <v>1.573799506506335</v>
+      </c>
+      <c r="D130">
+        <v>-1.866230480016994</v>
+      </c>
+      <c r="E130">
+        <v>-1.927404658431195</v>
+      </c>
+      <c r="F130">
+        <v>0.1140512787250589</v>
+      </c>
+      <c r="G130">
+        <v>-0.4685432583085821</v>
+      </c>
+      <c r="H130">
+        <v>-0.3728682174992243</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B131">
+        <v>1.563148290176452</v>
+      </c>
+      <c r="C131">
+        <v>-1.876881696346878</v>
+      </c>
+      <c r="D131">
+        <v>-1.938055874761079</v>
+      </c>
+      <c r="E131">
+        <v>0.1034000623951754</v>
+      </c>
+      <c r="F131">
+        <v>-0.4791944746384656</v>
+      </c>
+      <c r="G131">
+        <v>-0.3835194338291078</v>
+      </c>
+      <c r="H131">
+        <v>-0.6439384708278306</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B132">
+        <v>-1.985496228563019</v>
+      </c>
+      <c r="C132">
+        <v>-2.04667040697722</v>
+      </c>
+      <c r="D132">
+        <v>-0.005214469820965406</v>
+      </c>
+      <c r="E132">
+        <v>-0.5878090068546065</v>
+      </c>
+      <c r="F132">
+        <v>-0.4921339660452486</v>
+      </c>
+      <c r="G132">
+        <v>-0.7525530030439714</v>
+      </c>
+      <c r="H132">
+        <v>0.08290199311451979</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B133">
+        <v>-1.838568686009481</v>
+      </c>
+      <c r="C133">
+        <v>0.2028872511467736</v>
+      </c>
+      <c r="D133">
+        <v>-0.3797072858868674</v>
+      </c>
+      <c r="E133">
+        <v>-0.2840322450775096</v>
+      </c>
+      <c r="F133">
+        <v>-0.5444512820762324</v>
+      </c>
+      <c r="G133">
+        <v>0.2910037140822588</v>
+      </c>
+      <c r="H133">
+        <v>0.1909243541796373</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B134">
+        <v>0.319385421520574</v>
+      </c>
+      <c r="C134">
+        <v>-0.263209115513067</v>
+      </c>
+      <c r="D134">
+        <v>-0.1675340747037092</v>
+      </c>
+      <c r="E134">
+        <v>-0.427953111702432</v>
+      </c>
+      <c r="F134">
+        <v>0.4075018844560592</v>
+      </c>
+      <c r="G134">
+        <v>0.3074225245534377</v>
+      </c>
+      <c r="H134">
+        <v>-0.04636398152625851</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B135">
+        <v>-0.2177157015159319</v>
+      </c>
+      <c r="C135">
+        <v>-0.1220406607065741</v>
+      </c>
+      <c r="D135">
+        <v>-0.3824596977052969</v>
+      </c>
+      <c r="E135">
+        <v>0.4529952984531944</v>
+      </c>
+      <c r="F135">
+        <v>0.3529159385505728</v>
+      </c>
+      <c r="G135">
+        <v>-0.0008705675291234075</v>
+      </c>
+      <c r="H135">
+        <v>0.1473068229033219</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B136">
+        <v>-0.1395947820665385</v>
+      </c>
+      <c r="C136">
+        <v>-0.4000138190652613</v>
+      </c>
+      <c r="D136">
+        <v>0.4354411770932299</v>
+      </c>
+      <c r="E136">
+        <v>0.3353618171906084</v>
+      </c>
+      <c r="F136">
+        <v>-0.01842468888908786</v>
+      </c>
+      <c r="G136">
+        <v>0.1297527015433575</v>
+      </c>
+      <c r="H136">
+        <v>0.2871986905475125</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B137">
+        <v>-0.3119065001142551</v>
+      </c>
+      <c r="C137">
+        <v>0.5235484960442361</v>
+      </c>
+      <c r="D137">
+        <v>0.4234691361416146</v>
+      </c>
+      <c r="E137">
+        <v>0.06968263006191837</v>
+      </c>
+      <c r="F137">
+        <v>0.2178600204943637</v>
+      </c>
+      <c r="G137">
+        <v>0.3753060094985187</v>
+      </c>
+      <c r="H137">
+        <v>-0.1253534470275521</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B138">
+        <v>0.7021231295320197</v>
+      </c>
+      <c r="C138">
+        <v>0.6020437696293982</v>
+      </c>
+      <c r="D138">
+        <v>0.248257263549702</v>
+      </c>
+      <c r="E138">
+        <v>0.3964346539821473</v>
+      </c>
+      <c r="F138">
+        <v>0.5538806429863024</v>
+      </c>
+      <c r="G138">
+        <v>0.0532211864602315</v>
+      </c>
+      <c r="H138">
+        <v>0.3335790669957007</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B139">
+        <v>1.514070997382048</v>
+      </c>
+      <c r="C139">
+        <v>1.160284491302352</v>
+      </c>
+      <c r="D139">
+        <v>1.308461881734797</v>
+      </c>
+      <c r="E139">
+        <v>1.465907870738952</v>
+      </c>
+      <c r="F139">
+        <v>0.9652484142128814</v>
+      </c>
+      <c r="G139">
+        <v>1.245606294748351</v>
+      </c>
+      <c r="H139">
+        <v>1.073631436903339</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B140">
+        <v>0.2163102553365951</v>
+      </c>
+      <c r="C140">
+        <v>0.3644876457690405</v>
+      </c>
+      <c r="D140">
+        <v>0.5219336347731955</v>
+      </c>
+      <c r="E140">
+        <v>0.02127417824712469</v>
+      </c>
+      <c r="F140">
+        <v>0.3016320587825939</v>
+      </c>
+      <c r="G140">
+        <v>0.1296572009375822</v>
+      </c>
+      <c r="H140">
+        <v>0.4355197406839137</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B141">
+        <v>0.3684555432821496</v>
+      </c>
+      <c r="C141">
+        <v>0.5259015322863045</v>
+      </c>
+      <c r="D141">
+        <v>0.0252420757602338</v>
+      </c>
+      <c r="E141">
+        <v>0.305599956295703</v>
+      </c>
+      <c r="F141">
+        <v>0.1336250984506913</v>
+      </c>
+      <c r="G141">
+        <v>0.4394876381970228</v>
+      </c>
+      <c r="H141">
+        <v>-0.1728423144902634</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B142">
+        <v>0.661541622456546</v>
+      </c>
+      <c r="C142">
+        <v>0.1608821659304752</v>
+      </c>
+      <c r="D142">
+        <v>0.4412400464659443</v>
+      </c>
+      <c r="E142">
+        <v>0.2692651886209327</v>
+      </c>
+      <c r="F142">
+        <v>0.5751277283672642</v>
+      </c>
+      <c r="G142">
+        <v>-0.03720222432002201</v>
+      </c>
+      <c r="H142">
+        <v>0.6511691608790895</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B143">
+        <v>-0.07992401592518952</v>
+      </c>
+      <c r="C143">
+        <v>0.2004338646102796</v>
+      </c>
+      <c r="D143">
+        <v>0.028459006765268</v>
+      </c>
+      <c r="E143">
+        <v>0.3343215465115995</v>
+      </c>
+      <c r="F143">
+        <v>-0.2780084061756867</v>
+      </c>
+      <c r="G143">
+        <v>0.4103629790234248</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B144">
+        <v>0.1551026493581833</v>
+      </c>
+      <c r="C144">
+        <v>-0.01687220848682837</v>
+      </c>
+      <c r="D144">
+        <v>0.2889903312595031</v>
+      </c>
+      <c r="E144">
+        <v>-0.3233396214277831</v>
+      </c>
+      <c r="F144">
+        <v>0.3650317637713285</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B145">
+        <v>-0.08373363042288225</v>
+      </c>
+      <c r="C145">
+        <v>0.2221289093234493</v>
+      </c>
+      <c r="D145">
+        <v>-0.3902010433638369</v>
+      </c>
+      <c r="E145">
+        <v>0.2981703418352746</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B146">
+        <v>0.1925427069667326</v>
+      </c>
+      <c r="C146">
+        <v>-0.4197872457205535</v>
+      </c>
+      <c r="D146">
+        <v>0.268584139478558</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B147">
+        <v>-0.4379379024501944</v>
+      </c>
+      <c r="C147">
+        <v>0.2504334827489171</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B148">
         <v>0.2324016585002178</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>